<commit_message>
updates after pre-alpha run-through
</commit_message>
<xml_diff>
--- a/data/manual-data-example-01.xlsx
+++ b/data/manual-data-example-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob.harrand\OneDrive - Avacta Group plc\ANIMAL HEALTH\R Projects\life-sciences-spreadsheet-best-practice\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avactagroup-my.sharepoint.com/personal/rob_harrand_avacta_com1/Documents/ANIMAL HEALTH/R Projects/life-sciences-workshop/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:40009_{48510BBB-8B90-4451-BC63-28723668800B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BCC512F1-16AF-4484-8BB7-E22A10637839}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:40009_{48510BBB-8B90-4451-BC63-28723668800B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{60A872E6-CBD7-4E5C-A58A-9FCA4638E314}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27405" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>plate1</t>
   </si>
@@ -2193,10 +2193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,6 +2646,428 @@
         <v>9.2483530999999994E-2</v>
       </c>
     </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>11</v>
+      </c>
+      <c r="M15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>8.5020523834177242E-2</v>
+      </c>
+      <c r="C16">
+        <v>7.0018045722084574E-2</v>
+      </c>
+      <c r="D16">
+        <v>7.7347011281287431E-2</v>
+      </c>
+      <c r="E16">
+        <v>7.2985554110728754E-2</v>
+      </c>
+      <c r="F16">
+        <v>7.6163236380893437E-2</v>
+      </c>
+      <c r="G16">
+        <v>8.1312845846623127E-2</v>
+      </c>
+      <c r="H16">
+        <v>7.497706400245259E-2</v>
+      </c>
+      <c r="I16">
+        <v>6.799636856760724E-2</v>
+      </c>
+      <c r="J16">
+        <v>7.2554472448241009E-2</v>
+      </c>
+      <c r="K16">
+        <v>8.5848212023935042E-2</v>
+      </c>
+      <c r="L16">
+        <v>8.1620525404381999E-2</v>
+      </c>
+      <c r="M16">
+        <v>9.3042972978994415E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>6.580191817995007E-2</v>
+      </c>
+      <c r="C17">
+        <v>6.8591716791324767E-2</v>
+      </c>
+      <c r="D17">
+        <v>6.9584189478732281E-2</v>
+      </c>
+      <c r="E17">
+        <v>7.4870404963233453E-2</v>
+      </c>
+      <c r="F17">
+        <v>6.6398654032830962E-2</v>
+      </c>
+      <c r="G17">
+        <v>6.7099713926331517E-2</v>
+      </c>
+      <c r="H17">
+        <v>7.264508476042246E-2</v>
+      </c>
+      <c r="I17">
+        <v>7.2500740481186834E-2</v>
+      </c>
+      <c r="J17">
+        <v>6.8986735056413048E-2</v>
+      </c>
+      <c r="K17">
+        <v>7.1391480855683614E-2</v>
+      </c>
+      <c r="L17">
+        <v>7.4000346426255401E-2</v>
+      </c>
+      <c r="M17">
+        <v>8.5431274230973547E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>7.7572308016704589E-2</v>
+      </c>
+      <c r="C18">
+        <v>7.4973834760166669E-2</v>
+      </c>
+      <c r="D18">
+        <v>8.0104613468252622E-2</v>
+      </c>
+      <c r="E18">
+        <v>6.9326548289517329E-2</v>
+      </c>
+      <c r="F18">
+        <v>8.0448550559531942E-2</v>
+      </c>
+      <c r="G18">
+        <v>7.3346060114614198E-2</v>
+      </c>
+      <c r="H18">
+        <v>7.753446330252961E-2</v>
+      </c>
+      <c r="I18">
+        <v>6.9416288070665397E-2</v>
+      </c>
+      <c r="J18">
+        <v>6.7630354134056048E-2</v>
+      </c>
+      <c r="K18">
+        <v>7.4389420383033297E-2</v>
+      </c>
+      <c r="L18">
+        <v>6.5271202705754774E-2</v>
+      </c>
+      <c r="M18">
+        <v>7.7313392028465225E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>7.1848512219962357E-2</v>
+      </c>
+      <c r="C19">
+        <v>6.9568078340505116E-2</v>
+      </c>
+      <c r="D19">
+        <v>7.4743140980670059E-2</v>
+      </c>
+      <c r="E19">
+        <v>6.8000223885844965E-2</v>
+      </c>
+      <c r="F19">
+        <v>7.1424526617860709E-2</v>
+      </c>
+      <c r="G19">
+        <v>6.9259273552383482E-2</v>
+      </c>
+      <c r="H19">
+        <v>7.1474836758793237E-2</v>
+      </c>
+      <c r="I19">
+        <v>7.5083017522509121E-2</v>
+      </c>
+      <c r="J19">
+        <v>7.5745172459906612E-2</v>
+      </c>
+      <c r="K19">
+        <v>6.9658725335461094E-2</v>
+      </c>
+      <c r="L19">
+        <v>7.9051213740707088E-2</v>
+      </c>
+      <c r="M19">
+        <v>8.1530934618369966E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>6.9592024074287523E-2</v>
+      </c>
+      <c r="C20">
+        <v>7.3611351456340096E-2</v>
+      </c>
+      <c r="D20">
+        <v>7.1132565954102153E-2</v>
+      </c>
+      <c r="E20">
+        <v>7.1377739225816472E-2</v>
+      </c>
+      <c r="F20">
+        <v>6.7386650816961477E-2</v>
+      </c>
+      <c r="G20">
+        <v>7.5003470524710639E-2</v>
+      </c>
+      <c r="H20">
+        <v>8.0242786022444307E-2</v>
+      </c>
+      <c r="I20">
+        <v>7.3219868898411297E-2</v>
+      </c>
+      <c r="J20">
+        <v>7.1752687764215312E-2</v>
+      </c>
+      <c r="K20">
+        <v>7.1946319406849715E-2</v>
+      </c>
+      <c r="L20">
+        <v>7.6789404591961014E-2</v>
+      </c>
+      <c r="M20">
+        <v>7.4228397990308795E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>9.290608377263132E-2</v>
+      </c>
+      <c r="C21">
+        <v>0.10438887766531174</v>
+      </c>
+      <c r="D21">
+        <v>9.4250291386331009E-2</v>
+      </c>
+      <c r="E21">
+        <v>7.40263904168839E-2</v>
+      </c>
+      <c r="F21">
+        <v>7.6340170494104687E-2</v>
+      </c>
+      <c r="G21">
+        <v>7.056359159343592E-2</v>
+      </c>
+      <c r="H21">
+        <v>6.7197374143827343E-2</v>
+      </c>
+      <c r="I21">
+        <v>7.2270937357954132E-2</v>
+      </c>
+      <c r="J21">
+        <v>7.4207664270185408E-2</v>
+      </c>
+      <c r="K21">
+        <v>7.1215444955873619E-2</v>
+      </c>
+      <c r="L21">
+        <v>7.3014070176698656E-2</v>
+      </c>
+      <c r="M21">
+        <v>7.2655365685569517E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>7.8782578468679934E-2</v>
+      </c>
+      <c r="C22">
+        <v>8.1430808084095002E-2</v>
+      </c>
+      <c r="D22">
+        <v>7.2033306532744756E-2</v>
+      </c>
+      <c r="E22">
+        <v>7.5280110740534617E-2</v>
+      </c>
+      <c r="F22">
+        <v>8.0501507596732275E-2</v>
+      </c>
+      <c r="G22">
+        <v>7.5894447517653313E-2</v>
+      </c>
+      <c r="H22">
+        <v>7.3870048053369913E-2</v>
+      </c>
+      <c r="I22">
+        <v>7.215073276847532E-2</v>
+      </c>
+      <c r="J22">
+        <v>7.6221894123379666E-2</v>
+      </c>
+      <c r="K22">
+        <v>8.9920595852408677E-2</v>
+      </c>
+      <c r="L22">
+        <v>7.5665261649167842E-2</v>
+      </c>
+      <c r="M22">
+        <v>7.9714007508246754E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>7.9066285163548772E-2</v>
+      </c>
+      <c r="C23">
+        <v>7.7000012862131637E-2</v>
+      </c>
+      <c r="D23">
+        <v>8.2268654703213595E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.22722319391486348</v>
+      </c>
+      <c r="F23">
+        <v>0.27522216101230257</v>
+      </c>
+      <c r="G23">
+        <v>0.21467380024475677</v>
+      </c>
+      <c r="H23">
+        <v>9.465549729681523E-2</v>
+      </c>
+      <c r="I23">
+        <v>8.1983180650911827E-2</v>
+      </c>
+      <c r="J23">
+        <v>8.430083447225302E-2</v>
+      </c>
+      <c r="K23">
+        <v>9.1637984998670846E-2</v>
+      </c>
+      <c r="L23">
+        <v>9.633838338134354E-2</v>
+      </c>
+      <c r="M23">
+        <v>9.7500349239445089E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25">
+        <f>MAX(B16:B23)</f>
+        <v>9.290608377263132E-2</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:M25" si="1">MAX(C16:C23)</f>
+        <v>0.10438887766531174</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>9.4250291386331009E-2</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0.22722319391486348</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0.27522216101230257</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0.21467380024475677</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>9.465549729681523E-2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>8.1983180650911827E-2</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>8.430083447225302E-2</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>9.1637984998670846E-2</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>9.633838338134354E-2</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>9.7500349239445089E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2655,8 +3077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5617,6 +6039,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004DB9F5D92B7EB6498533E14AA62F30E0" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20fe52a65a6fbd0a4766a2e26df7d6fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3c531925-a8e9-4f82-822f-6e720afa08d7" xmlns:ns4="8698945b-6f9d-463e-b0af-88f8ba16812e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ec4227a4fb91e11e9f671e1cfe49db7" ns3:_="" ns4:_="">
     <xsd:import namespace="3c531925-a8e9-4f82-822f-6e720afa08d7"/>
@@ -5825,36 +6262,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F80C11B-F8C4-47B0-A4F5-5108F9969AF8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806CDB68-30E0-4B08-ABC4-2B53278CFA2D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3c531925-a8e9-4f82-822f-6e720afa08d7"/>
-    <ds:schemaRef ds:uri="8698945b-6f9d-463e-b0af-88f8ba16812e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5877,9 +6288,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806CDB68-30E0-4B08-ABC4-2B53278CFA2D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F80C11B-F8C4-47B0-A4F5-5108F9969AF8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3c531925-a8e9-4f82-822f-6e720afa08d7"/>
+    <ds:schemaRef ds:uri="8698945b-6f9d-463e-b0af-88f8ba16812e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>